<commit_message>
functional test to check when an offer is changed (quantity is increased) and someone else sells part or all of it before the form is submitted. Views.py code tidy up.
</commit_message>
<xml_diff>
--- a/proj_aged/core/aged/lab/DataSafeOnes/18_just_three_sales_people.xlsx
+++ b/proj_aged/core/aged/lab/DataSafeOnes/18_just_three_sales_people.xlsx
@@ -1302,10 +1302,10 @@
   <dimension ref="B1:E375"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A175" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B212" activeCellId="0" sqref="B212"/>
+      <selection pane="topLeft" activeCell="B178" activeCellId="0" sqref="B178"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>

</xml_diff>